<commit_message>
Pridane SubjectTerm, MilestoneResult,este bez kontrollers a services
</commit_message>
<xml_diff>
--- a/doc/studenture db.xlsx
+++ b/doc/studenture db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anita\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA462819-F12E-4C7A-B509-EB52DC238F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D872ADBC-97BD-4891-B05B-47593FD764DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>nazov table</t>
   </si>
@@ -122,9 +122,6 @@
     <t>semester</t>
   </si>
   <si>
-    <t>ExamResult</t>
-  </si>
-  <si>
     <t>RecordCard</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
     <t>milestone_maximum</t>
   </si>
   <si>
-    <t>student_name</t>
-  </si>
-  <si>
-    <t>exam_result</t>
-  </si>
-  <si>
-    <t>HashMap&lt;Student, List&lt;ExamResult&gt;&gt;</t>
-  </si>
-  <si>
     <t>subject_credits</t>
   </si>
   <si>
@@ -197,29 +185,41 @@
     <t>List&lt;Milestone&gt;</t>
   </si>
   <si>
-    <t>one-to many</t>
-  </si>
-  <si>
-    <t>many-to one</t>
-  </si>
-  <si>
     <t>long</t>
   </si>
   <si>
-    <t>table</t>
-  </si>
-  <si>
     <t>List&lt;SubjectTerm&gt;</t>
   </si>
   <si>
     <t>many-to-many</t>
+  </si>
+  <si>
+    <t>subject_result</t>
+  </si>
+  <si>
+    <t>many-to many</t>
+  </si>
+  <si>
+    <t>mal by prepočitat sumar z List&lt;Milestone&gt; milestone_result</t>
+  </si>
+  <si>
+    <t>a porovnat ich s subject_credits</t>
+  </si>
+  <si>
+    <t>kontola ze milestone_result je &lt;=milestone.maximum</t>
+  </si>
+  <si>
+    <t>prepojenie cez subjectterm_milestones</t>
+  </si>
+  <si>
+    <t>table este je nedokoncena v db</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +254,29 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -261,12 +284,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -280,8 +297,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -289,20 +312,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -583,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +639,8 @@
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="6" max="6" width="57" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,133 +701,140 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -792,55 +844,58 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="G25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -849,15 +904,15 @@
       <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K26" s="6"/>
+      <c r="G26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -866,113 +921,116 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="6"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6" t="s">
+      <c r="C29" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F31" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>44</v>
+      <c r="B32" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" t="s">
         <v>3</v>
       </c>
+      <c r="C34" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="B35" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="B36" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="B38" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
       <c r="F38" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>34</v>
-      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>